<commit_message>
Bug fix update 2024
</commit_message>
<xml_diff>
--- a/Examples/Graphics/test.xlsx
+++ b/Examples/Graphics/test.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26731"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Matlab\Utvikling\MATLAB_LIB\NBTOOLBOX\Examples\Graphics\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="P:\Matlab\Utvikling\MATLAB_LIB\NBTOOLBOX\Examples\Graphics\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{81523656-0954-431D-BEF8-840A527FFEC0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="38380" windowHeight="6610"/>
+    <workbookView xWindow="1170" yWindow="1170" windowWidth="21600" windowHeight="11325" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
   <si>
     <t>Var1</t>
   </si>
@@ -33,12 +34,60 @@
   </si>
   <si>
     <t>Time</t>
+  </si>
+  <si>
+    <t>01.01.2001</t>
+  </si>
+  <si>
+    <t>01.04.2001</t>
+  </si>
+  <si>
+    <t>01.07.2001</t>
+  </si>
+  <si>
+    <t>01.10.2001</t>
+  </si>
+  <si>
+    <t>01.01.2002</t>
+  </si>
+  <si>
+    <t>01.04.2002</t>
+  </si>
+  <si>
+    <t>01.07.2002</t>
+  </si>
+  <si>
+    <t>01.10.2002</t>
+  </si>
+  <si>
+    <t>01.01.2003</t>
+  </si>
+  <si>
+    <t>01.04.2003</t>
+  </si>
+  <si>
+    <t>01.07.2003</t>
+  </si>
+  <si>
+    <t>01.10.2003</t>
+  </si>
+  <si>
+    <t>01.01.2004</t>
+  </si>
+  <si>
+    <t>01.04.2004</t>
+  </si>
+  <si>
+    <t>01.07.2004</t>
+  </si>
+  <si>
+    <t>01.10.2004</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -350,16 +399,16 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection sqref="A1:C17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>2</v>
       </c>
@@ -370,9 +419,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A2" s="1">
-        <v>36892</v>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>3</v>
       </c>
       <c r="B2">
         <v>0.98406372437915379</v>
@@ -381,9 +430,9 @@
         <v>0.53912646504285666</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A3" s="1">
-        <v>36982</v>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>4</v>
       </c>
       <c r="B3">
         <v>0.16716840991465598</v>
@@ -392,9 +441,9 @@
         <v>0.69810552018030836</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A4" s="1">
-        <v>37073</v>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>5</v>
       </c>
       <c r="B4">
         <v>0.10621634492866383</v>
@@ -403,9 +452,9 @@
         <v>0.66652791340258688</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A5" s="1">
-        <v>37165</v>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>6</v>
       </c>
       <c r="B5">
         <v>0.37240974005553695</v>
@@ -414,9 +463,9 @@
         <v>0.17813245440033776</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A6" s="1">
-        <v>37257</v>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>7</v>
       </c>
       <c r="B6">
         <v>0.19811840254297464</v>
@@ -425,9 +474,9 @@
         <v>0.12801439972017259</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A7" s="1">
-        <v>37347</v>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
+        <v>8</v>
       </c>
       <c r="B7">
         <v>0.48968763801602389</v>
@@ -436,9 +485,9 @@
         <v>0.99908039476136068</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A8" s="1">
-        <v>37438</v>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
+        <v>9</v>
       </c>
       <c r="B8">
         <v>0.33949341339075767</v>
@@ -447,9 +496,9 @@
         <v>0.17112106635643209</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A9" s="1">
-        <v>37530</v>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
+        <v>10</v>
       </c>
       <c r="B9">
         <v>0.95163046477772695</v>
@@ -458,9 +507,9 @@
         <v>3.2600820530528041E-2</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A10" s="1">
-        <v>37622</v>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
+        <v>11</v>
       </c>
       <c r="B10">
         <v>0.92033203983656375</v>
@@ -469,9 +518,9 @@
         <v>0.56119979270966014</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A11" s="1">
-        <v>37712</v>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
+        <v>12</v>
       </c>
       <c r="B11">
         <v>5.2676997680792592E-2</v>
@@ -480,9 +529,9 @@
         <v>0.88186650045180992</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A12" s="1">
-        <v>37803</v>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12" s="1" t="s">
+        <v>13</v>
       </c>
       <c r="B12">
         <v>0.73785809551699655</v>
@@ -491,9 +540,9 @@
         <v>0.66917530453439378</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A13" s="1">
-        <v>37895</v>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13" s="1" t="s">
+        <v>14</v>
       </c>
       <c r="B13">
         <v>0.26911942639855591</v>
@@ -502,9 +551,9 @@
         <v>0.19043326717995412</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A14" s="1">
-        <v>37987</v>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14" s="1" t="s">
+        <v>15</v>
       </c>
       <c r="B14">
         <v>0.42283561500880784</v>
@@ -513,9 +562,9 @@
         <v>0.3689165460638949</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A15" s="1">
-        <v>38078</v>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A15" s="1" t="s">
+        <v>16</v>
       </c>
       <c r="B15">
         <v>0.54787090121484472</v>
@@ -524,9 +573,9 @@
         <v>0.46072593726041156</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A16" s="1">
-        <v>38169</v>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A16" s="1" t="s">
+        <v>17</v>
       </c>
       <c r="B16">
         <v>0.94273698427693431</v>
@@ -535,9 +584,9 @@
         <v>0.98163795097074968</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A17" s="1">
-        <v>38261</v>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17" s="1" t="s">
+        <v>18</v>
       </c>
       <c r="B17">
         <v>0.4177441043166622</v>
@@ -546,7 +595,7 @@
         <v>0.15640495222656348</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>19</v>
       </c>
@@ -557,7 +606,7 @@
         <v>0.57852506102343892</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>20</v>
       </c>

</xml_diff>